<commit_message>
Fixed error where species was missing data
</commit_message>
<xml_diff>
--- a/data/Detailed_methods.xlsx
+++ b/data/Detailed_methods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/usr/local/bin/store/partner_rff/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2649B9A5-5F12-0E4C-A488-862AEEBFC455}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EFD3D3-05CB-C14D-AB43-3E2504704985}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="460" windowWidth="24640" windowHeight="13740" xr2:uid="{804B5181-2E36-0144-BC00-F5005385D24D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2462" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2460" uniqueCount="784">
   <si>
     <t>Scientific name</t>
   </si>
@@ -2844,8 +2844,8 @@
   <dimension ref="A1:XDX142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -41726,12 +41726,6 @@
       <c r="AA82" t="s">
         <v>727</v>
       </c>
-      <c r="AB82" t="s">
-        <v>704</v>
-      </c>
-      <c r="AC82">
-        <v>2</v>
-      </c>
       <c r="AD82" s="9"/>
     </row>
     <row r="83" spans="1:30">
@@ -41815,10 +41809,10 @@
         <v>763</v>
       </c>
       <c r="AB83" t="s">
-        <v>301</v>
-      </c>
-      <c r="AC83" t="s">
-        <v>301</v>
+        <v>704</v>
+      </c>
+      <c r="AC83" s="9">
+        <v>2</v>
       </c>
       <c r="AD83" s="9"/>
     </row>

</xml_diff>

<commit_message>
new figured made and added to folder for thesis Also went through and highlighted missing documents in Detailed_methods when I was downloading pdfs
</commit_message>
<xml_diff>
--- a/data/Detailed_methods.xlsx
+++ b/data/Detailed_methods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/usr/local/bin/store/partner_rff/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EFD3D3-05CB-C14D-AB43-3E2504704985}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703B31EA-D5CB-C042-96ED-3935DD0B4990}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="460" windowWidth="24640" windowHeight="13740" xr2:uid="{804B5181-2E36-0144-BC00-F5005385D24D}"/>
+    <workbookView xWindow="1060" yWindow="2360" windowWidth="24640" windowHeight="13740" xr2:uid="{804B5181-2E36-0144-BC00-F5005385D24D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2460" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2459" uniqueCount="784">
   <si>
     <t>Scientific name</t>
   </si>
@@ -2438,7 +2438,7 @@
       <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2481,6 +2481,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEA423E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2495,7 +2507,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -2526,6 +2538,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2533,6 +2551,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEA423E"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2844,8 +2867,8 @@
   <dimension ref="A1:XDX142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F83" sqref="F83"/>
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H125" sqref="H125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3194,30 +3217,15 @@
       </c>
     </row>
     <row r="5" spans="1:16352">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>580</v>
-      </c>
-      <c r="D5" t="s">
-        <v>321</v>
-      </c>
-      <c r="F5" t="s">
-        <v>610</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>331</v>
-      </c>
+      <c r="A5" s="9"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
       <c r="J5" t="s">
         <v>177</v>
       </c>
@@ -3266,9 +3274,29 @@
       <c r="Y5" s="4"/>
     </row>
     <row r="6" spans="1:16352">
-      <c r="B6" s="1"/>
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C6" t="s">
-        <v>177</v>
+        <v>580</v>
+      </c>
+      <c r="D6" t="s">
+        <v>321</v>
+      </c>
+      <c r="F6" t="s">
+        <v>610</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>331</v>
       </c>
       <c r="J6" t="s">
         <v>177</v>
@@ -39766,7 +39794,7 @@
       <c r="L57" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="M57" s="14" t="s">
+      <c r="M57" s="21" t="s">
         <v>478</v>
       </c>
       <c r="N57" s="9" t="s">
@@ -40179,13 +40207,13 @@
       <c r="K62" t="s">
         <v>450</v>
       </c>
-      <c r="L62" s="9" t="s">
+      <c r="L62" s="28" t="s">
         <v>452</v>
       </c>
-      <c r="M62" s="9" t="s">
+      <c r="M62" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="N62" s="9" t="s">
+      <c r="N62" s="28" t="s">
         <v>301</v>
       </c>
       <c r="O62" s="9">
@@ -40260,13 +40288,13 @@
       <c r="J63" t="s">
         <v>177</v>
       </c>
-      <c r="L63" s="9" t="s">
+      <c r="L63" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="M63" s="14" t="s">
+      <c r="M63" s="21" t="s">
         <v>476</v>
       </c>
-      <c r="N63" s="9" t="s">
+      <c r="N63" s="28" t="s">
         <v>387</v>
       </c>
       <c r="O63" s="9">
@@ -40996,11 +41024,11 @@
         <v>177</v>
       </c>
       <c r="K73" s="12"/>
-      <c r="L73" s="14"/>
-      <c r="M73" s="14" t="s">
+      <c r="L73" s="29"/>
+      <c r="M73" s="29" t="s">
         <v>258</v>
       </c>
-      <c r="N73" s="9" t="s">
+      <c r="N73" s="30" t="s">
         <v>299</v>
       </c>
       <c r="O73" s="9">
@@ -41410,13 +41438,13 @@
       <c r="K78" t="s">
         <v>599</v>
       </c>
-      <c r="L78" s="9" t="s">
+      <c r="L78" s="30" t="s">
         <v>485</v>
       </c>
-      <c r="M78" s="14" t="s">
+      <c r="M78" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="N78" s="9" t="s">
+      <c r="N78" s="30" t="s">
         <v>301</v>
       </c>
       <c r="O78" s="9">
@@ -41760,13 +41788,13 @@
       <c r="K83" s="12" t="s">
         <v>704</v>
       </c>
-      <c r="L83" s="9" t="s">
+      <c r="L83" s="28" t="s">
         <v>703</v>
       </c>
-      <c r="M83" s="16" t="s">
+      <c r="M83" s="31" t="s">
         <v>269</v>
       </c>
-      <c r="N83" s="9" t="s">
+      <c r="N83" s="28" t="s">
         <v>301</v>
       </c>
       <c r="O83" s="9">
@@ -42129,7 +42157,7 @@
       <c r="L88" s="20" t="s">
         <v>510</v>
       </c>
-      <c r="M88" s="14" t="s">
+      <c r="M88" s="21" t="s">
         <v>225</v>
       </c>
       <c r="N88" s="9" t="s">
@@ -42175,7 +42203,7 @@
       <c r="L89" s="19" t="s">
         <v>508</v>
       </c>
-      <c r="M89" s="14" t="s">
+      <c r="M89" s="21" t="s">
         <v>272</v>
       </c>
       <c r="N89" s="9" t="s">
@@ -42329,7 +42357,7 @@
       <c r="L91" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="M91" s="10" t="s">
+      <c r="M91" s="21" t="s">
         <v>275</v>
       </c>
       <c r="N91" s="6" t="s">
@@ -42777,13 +42805,13 @@
       <c r="J98" t="s">
         <v>177</v>
       </c>
-      <c r="L98" s="9" t="s">
+      <c r="L98" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="M98" s="10" t="s">
+      <c r="M98" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="N98" s="9" t="s">
+      <c r="N98" s="28" t="s">
         <v>387</v>
       </c>
       <c r="O98" s="9">
@@ -43118,13 +43146,13 @@
       <c r="I103" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L103" s="9" t="s">
+      <c r="L103" s="32" t="s">
         <v>548</v>
       </c>
-      <c r="M103" s="10" t="s">
+      <c r="M103" s="33" t="s">
         <v>549</v>
       </c>
-      <c r="N103" s="9" t="s">
+      <c r="N103" s="32" t="s">
         <v>192</v>
       </c>
       <c r="O103" s="9">
@@ -43865,10 +43893,11 @@
       <c r="C114" t="s">
         <v>177</v>
       </c>
-      <c r="M114" s="10" t="s">
+      <c r="L114" s="28"/>
+      <c r="M114" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="N114" s="9" t="s">
+      <c r="N114" s="28" t="s">
         <v>387</v>
       </c>
       <c r="O114" s="9">
@@ -44164,13 +44193,13 @@
       <c r="K118" t="s">
         <v>530</v>
       </c>
-      <c r="L118" s="9" t="s">
+      <c r="L118" s="28" t="s">
         <v>568</v>
       </c>
-      <c r="M118" s="10" t="s">
+      <c r="M118" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="N118" s="9" t="s">
+      <c r="N118" s="28" t="s">
         <v>301</v>
       </c>
       <c r="O118" s="9">

</xml_diff>